<commit_message>
Updating Intervention content and delivery.xlsx
</commit_message>
<xml_diff>
--- a/Intervention content and delivery/Intervention content and delivery.xlsx
+++ b/Intervention content and delivery/Intervention content and delivery.xlsx
@@ -777,62 +777,62 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>GMHO:0000001</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>dose of pharmacological substance</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Dose of pharmacological substance delivered to an individual.</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>dose</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr"/>
-      <c r="G6" s="2" t="inlineStr"/>
-      <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="inlineStr"/>
-      <c r="J6" s="2" t="inlineStr"/>
-      <c r="K6" s="2" t="inlineStr"/>
-      <c r="L6" s="2" t="inlineStr"/>
-      <c r="M6" s="2" t="inlineStr"/>
-      <c r="N6" s="2" t="inlineStr"/>
-      <c r="O6" s="2" t="inlineStr"/>
-      <c r="P6" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q6" s="2" t="inlineStr">
-        <is>
-          <t>Intervention content and delivery</t>
-        </is>
-      </c>
-      <c r="R6" s="2" t="inlineStr"/>
-      <c r="S6" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T6" s="2" t="inlineStr"/>
-      <c r="U6" s="2" t="inlineStr">
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Intervention content and delivery</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
         <is>
           <t>external parent class needs to be represented on Github spreadsheet for external entities</t>
         </is>
       </c>
-      <c r="V6" s="2" t="inlineStr">
-        <is>
-          <t>PS</t>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>PS; BG</t>
         </is>
       </c>
     </row>

</xml_diff>